<commit_message>
Got Data from PDF 20 and 22
</commit_message>
<xml_diff>
--- a/Results_data_all.xlsx
+++ b/Results_data_all.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5304" uniqueCount="1907">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5321" uniqueCount="1924">
   <si>
     <t>V1</t>
   </si>
@@ -5747,6 +5747,57 @@
   </si>
   <si>
     <t>Soil 1999-105_MAD</t>
+  </si>
+  <si>
+    <t>SRS1311</t>
+  </si>
+  <si>
+    <t>SRS1312</t>
+  </si>
+  <si>
+    <t>SRS1313</t>
+  </si>
+  <si>
+    <t>SRS1314</t>
+  </si>
+  <si>
+    <t>SRS1315</t>
+  </si>
+  <si>
+    <t>SRS1301</t>
+  </si>
+  <si>
+    <t>SRS1302</t>
+  </si>
+  <si>
+    <t>SRS1303</t>
+  </si>
+  <si>
+    <t>SRS1304</t>
+  </si>
+  <si>
+    <t>SRS1305</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>Sand_Mean</t>
+  </si>
+  <si>
+    <t>Sand_MAD</t>
+  </si>
+  <si>
+    <t>Silt_Mean</t>
+  </si>
+  <si>
+    <t>Silt_MAD</t>
+  </si>
+  <si>
+    <t>Clay_Mean</t>
+  </si>
+  <si>
+    <t>Clay_MAD</t>
   </si>
 </sst>
 </file>
@@ -45340,14 +45391,276 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C4"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1917</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1918</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1920</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1921</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1922</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1923</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1907</v>
+      </c>
+      <c r="B2">
+        <v>47</v>
+      </c>
+      <c r="C2">
+        <v>5.3</v>
+      </c>
+      <c r="D2">
+        <v>40</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>14.7</v>
+      </c>
+      <c r="G2">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1908</v>
+      </c>
+      <c r="B3">
+        <v>45.7</v>
+      </c>
+      <c r="C3">
+        <v>5.3</v>
+      </c>
+      <c r="D3">
+        <v>44.7</v>
+      </c>
+      <c r="E3">
+        <v>4.7</v>
+      </c>
+      <c r="F3">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1909</v>
+      </c>
+      <c r="B4">
+        <v>92.9</v>
+      </c>
+      <c r="C4">
+        <v>1.8</v>
+      </c>
+      <c r="D4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E4">
+        <v>0.83</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1910</v>
+      </c>
+      <c r="B5">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>3.6</v>
+      </c>
+      <c r="D5">
+        <v>36</v>
+      </c>
+      <c r="E5">
+        <v>3.2</v>
+      </c>
+      <c r="F5">
+        <v>36</v>
+      </c>
+      <c r="G5">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1911</v>
+      </c>
+      <c r="B6">
+        <v>9.58</v>
+      </c>
+      <c r="C6">
+        <v>2.92</v>
+      </c>
+      <c r="D6">
+        <v>66</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>23</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B7">
+        <v>94.3</v>
+      </c>
+      <c r="C7">
+        <v>1.5</v>
+      </c>
+      <c r="D7">
+        <v>2.59</v>
+      </c>
+      <c r="E7">
+        <v>0.59</v>
+      </c>
+      <c r="F7">
+        <v>3.5</v>
+      </c>
+      <c r="G7">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1913</v>
+      </c>
+      <c r="B8">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="C8">
+        <v>2.5</v>
+      </c>
+      <c r="D8">
+        <v>22</v>
+      </c>
+      <c r="E8">
+        <v>1.9</v>
+      </c>
+      <c r="F8">
+        <v>10.7</v>
+      </c>
+      <c r="G8">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1914</v>
+      </c>
+      <c r="B9">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="C9">
+        <v>3.5</v>
+      </c>
+      <c r="D9">
+        <v>22.5</v>
+      </c>
+      <c r="E9">
+        <v>1.7</v>
+      </c>
+      <c r="F9">
+        <v>6.3</v>
+      </c>
+      <c r="G9">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B10">
+        <v>44.7</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>31.2</v>
+      </c>
+      <c r="E10">
+        <v>4.7</v>
+      </c>
+      <c r="F10">
+        <v>24.6</v>
+      </c>
+      <c r="G10">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1916</v>
+      </c>
+      <c r="B11">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>52</v>
+      </c>
+      <c r="E11">
+        <v>2.1</v>
+      </c>
+      <c r="F11">
+        <v>9.83</v>
+      </c>
+      <c r="G11">
+        <v>1.07</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updates and new code for different formats
</commit_message>
<xml_diff>
--- a/Results_data_all.xlsx
+++ b/Results_data_all.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Results_data_all" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5321" uniqueCount="1924">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5382" uniqueCount="1985">
   <si>
     <t>V1</t>
   </si>
@@ -5798,6 +5798,189 @@
   </si>
   <si>
     <t>Clay_MAD</t>
+  </si>
+  <si>
+    <t>SRSSRS1306</t>
+  </si>
+  <si>
+    <t>SRSSRS1307</t>
+  </si>
+  <si>
+    <t>SRSSRS1308</t>
+  </si>
+  <si>
+    <t>SRSSRS1309</t>
+  </si>
+  <si>
+    <t>SRSSRS1310</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRS1401</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRS1402</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRS1403</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRS1404</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRS1405</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1411</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1412</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1413</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1414</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1415</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1501</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1502</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1503</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1504</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1505</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1506</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1507</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1508</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1509</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1510</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1511</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1512</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1513</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1514</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1515</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1601</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1602</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1603</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1604</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1605</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1606</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1607</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1608</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1609</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SRSSRS1610</t>
+  </si>
+  <si>
+    <t>SRS1611</t>
+  </si>
+  <si>
+    <t>SRS1613</t>
+  </si>
+  <si>
+    <t>SRS1614</t>
+  </si>
+  <si>
+    <t>SRS1615</t>
+  </si>
+  <si>
+    <t>SSR1612</t>
+  </si>
+  <si>
+    <t>SRS1701</t>
+  </si>
+  <si>
+    <t>SRS1702</t>
+  </si>
+  <si>
+    <t>SRS1703</t>
+  </si>
+  <si>
+    <t>SRS1704</t>
+  </si>
+  <si>
+    <t>SRS1705</t>
+  </si>
+  <si>
+    <t>SRS1706</t>
+  </si>
+  <si>
+    <t>SRS1707</t>
+  </si>
+  <si>
+    <t>SRS1708</t>
+  </si>
+  <si>
+    <t>SRS1709</t>
+  </si>
+  <si>
+    <t>SRS1710</t>
+  </si>
+  <si>
+    <t>SRS1711</t>
+  </si>
+  <si>
+    <t>SRS1712</t>
+  </si>
+  <si>
+    <t>SRS1713</t>
+  </si>
+  <si>
+    <t>SRS1714</t>
+  </si>
+  <si>
+    <t>SRS1715</t>
   </si>
 </sst>
 </file>
@@ -5807,7 +5990,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -5836,6 +6019,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -5878,7 +6067,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2249">
+  <cellXfs count="2250">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1">
@@ -12608,6 +12797,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12896,7 +13088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M658"/>
   <sheetViews>
-    <sheetView topLeftCell="B651" workbookViewId="0">
+    <sheetView topLeftCell="B627" workbookViewId="0">
       <selection activeCell="F161" sqref="F161:I658"/>
     </sheetView>
   </sheetViews>
@@ -30974,7 +31166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
+    <sheetView topLeftCell="A94" workbookViewId="0">
       <selection activeCell="D111" sqref="A3:D111"/>
     </sheetView>
   </sheetViews>
@@ -32546,7 +32738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G300"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -45391,15 +45583,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="I66" sqref="I66:I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -45407,7 +45599,7 @@
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1917</v>
       </c>
@@ -45429,8 +45621,11 @@
       <c r="G1" t="s">
         <v>1923</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>1934</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1907</v>
       </c>
@@ -45452,8 +45647,12 @@
       <c r="G2">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <f>B2+D2+F2</f>
+        <v>101.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1908</v>
       </c>
@@ -45475,8 +45674,12 @@
       <c r="G3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <f t="shared" ref="I3:I67" si="0">B3+D3+F3</f>
+        <v>98.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1909</v>
       </c>
@@ -45498,8 +45701,12 @@
       <c r="G4">
         <v>1.21</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>100.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1910</v>
       </c>
@@ -45521,8 +45728,12 @@
       <c r="G5">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1911</v>
       </c>
@@ -45544,8 +45755,12 @@
       <c r="G6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>98.58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1912</v>
       </c>
@@ -45567,8 +45782,12 @@
       <c r="G7">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>100.39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1913</v>
       </c>
@@ -45590,8 +45809,12 @@
       <c r="G8">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>101.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1914</v>
       </c>
@@ -45613,8 +45836,12 @@
       <c r="G9">
         <v>1.1299999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>100.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1915</v>
       </c>
@@ -45636,8 +45863,12 @@
       <c r="G10">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>100.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1916</v>
       </c>
@@ -45659,9 +45890,1634 @@
       <c r="G11">
         <v>1.07</v>
       </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>102.53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1924</v>
+      </c>
+      <c r="B12">
+        <v>67</v>
+      </c>
+      <c r="C12">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D12">
+        <v>24.5</v>
+      </c>
+      <c r="E12">
+        <v>3.2</v>
+      </c>
+      <c r="F12">
+        <v>5.67</v>
+      </c>
+      <c r="G12">
+        <v>2.83</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>97.17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1925</v>
+      </c>
+      <c r="B13">
+        <v>66.7</v>
+      </c>
+      <c r="C13">
+        <v>1.7</v>
+      </c>
+      <c r="D13">
+        <v>24.8</v>
+      </c>
+      <c r="E13">
+        <v>2.7</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <v>2.33</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>101.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1926</v>
+      </c>
+      <c r="B14">
+        <v>25.3</v>
+      </c>
+      <c r="C14">
+        <v>2.7</v>
+      </c>
+      <c r="D14">
+        <v>39.5</v>
+      </c>
+      <c r="E14">
+        <v>1.7</v>
+      </c>
+      <c r="F14">
+        <v>36</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>100.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1927</v>
+      </c>
+      <c r="B15">
+        <v>84.7</v>
+      </c>
+      <c r="C15">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D15">
+        <v>6.4</v>
+      </c>
+      <c r="E15">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="F15">
+        <v>9</v>
+      </c>
+      <c r="G15">
+        <v>1.67</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>100.10000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1928</v>
+      </c>
+      <c r="B16">
+        <v>66.5</v>
+      </c>
+      <c r="C16">
+        <v>2.5</v>
+      </c>
+      <c r="D16">
+        <v>19.7</v>
+      </c>
+      <c r="E16">
+        <v>1.7</v>
+      </c>
+      <c r="F16">
+        <v>14.3</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>100.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1929</v>
+      </c>
+      <c r="B17">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="C17">
+        <v>2.4</v>
+      </c>
+      <c r="D17">
+        <v>68.5</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>14.8</v>
+      </c>
+      <c r="G17">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>101.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1930</v>
+      </c>
+      <c r="B18">
+        <v>50.2</v>
+      </c>
+      <c r="C18">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D18">
+        <v>36.6</v>
+      </c>
+      <c r="E18">
+        <v>2.5</v>
+      </c>
+      <c r="F18">
+        <v>14.5</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>101.30000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1931</v>
+      </c>
+      <c r="B19">
+        <v>79.8</v>
+      </c>
+      <c r="C19">
+        <v>1.8</v>
+      </c>
+      <c r="D19">
+        <v>12</v>
+      </c>
+      <c r="E19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F19">
+        <v>8.83</v>
+      </c>
+      <c r="G19">
+        <v>0.97</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>100.63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B20">
+        <v>44.4</v>
+      </c>
+      <c r="C20">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D20">
+        <v>40</v>
+      </c>
+      <c r="E20">
+        <v>2.8</v>
+      </c>
+      <c r="F20">
+        <v>16.8</v>
+      </c>
+      <c r="G20">
+        <v>1.6</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>101.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1933</v>
+      </c>
+      <c r="B21">
+        <v>81</v>
+      </c>
+      <c r="C21">
+        <v>1.4</v>
+      </c>
+      <c r="D21">
+        <v>11.9</v>
+      </c>
+      <c r="E21">
+        <v>1.3</v>
+      </c>
+      <c r="F21">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="G21">
+        <v>1.37</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>101.02000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1935</v>
+      </c>
+      <c r="B22">
+        <v>63.7</v>
+      </c>
+      <c r="C22">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D22">
+        <v>28</v>
+      </c>
+      <c r="E22">
+        <v>1.9</v>
+      </c>
+      <c r="F22">
+        <v>7.13</v>
+      </c>
+      <c r="G22">
+        <v>2.25</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>98.83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1936</v>
+      </c>
+      <c r="B23">
+        <v>51</v>
+      </c>
+      <c r="C23">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D23">
+        <v>36.9</v>
+      </c>
+      <c r="E23">
+        <v>2.7</v>
+      </c>
+      <c r="F23">
+        <v>12.7</v>
+      </c>
+      <c r="G23">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>100.60000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1937</v>
+      </c>
+      <c r="B24">
+        <v>34.6</v>
+      </c>
+      <c r="C24">
+        <v>3.4</v>
+      </c>
+      <c r="D24">
+        <v>49.9</v>
+      </c>
+      <c r="E24">
+        <v>3.8</v>
+      </c>
+      <c r="F24">
+        <v>13.3</v>
+      </c>
+      <c r="G24">
+        <v>3.9</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>97.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1938</v>
+      </c>
+      <c r="B25">
+        <v>14.4</v>
+      </c>
+      <c r="C25">
+        <v>4.3</v>
+      </c>
+      <c r="D25">
+        <v>50</v>
+      </c>
+      <c r="E25">
+        <v>3.9</v>
+      </c>
+      <c r="F25">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="G25">
+        <v>2.7</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>97.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1939</v>
+      </c>
+      <c r="B26">
+        <v>37.1</v>
+      </c>
+      <c r="C26">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D26">
+        <v>31.5</v>
+      </c>
+      <c r="E26">
+        <v>2.8</v>
+      </c>
+      <c r="F26">
+        <v>31.8</v>
+      </c>
+      <c r="G26">
+        <v>2.6</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>100.39999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1940</v>
+      </c>
+      <c r="B27">
+        <v>49.2</v>
+      </c>
+      <c r="C27">
+        <v>2.8</v>
+      </c>
+      <c r="D27">
+        <v>34.4</v>
+      </c>
+      <c r="E27">
+        <v>3.1</v>
+      </c>
+      <c r="F27">
+        <v>16.8</v>
+      </c>
+      <c r="G27">
+        <v>3.3</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>100.39999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1941</v>
+      </c>
+      <c r="B28">
+        <v>12.7</v>
+      </c>
+      <c r="C28">
+        <v>2.7</v>
+      </c>
+      <c r="D28">
+        <v>55.9</v>
+      </c>
+      <c r="E28">
+        <v>4.5</v>
+      </c>
+      <c r="F28">
+        <v>31.9</v>
+      </c>
+      <c r="G28">
+        <v>1.9</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>100.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1942</v>
+      </c>
+      <c r="B29">
+        <v>87</v>
+      </c>
+      <c r="C29">
+        <v>1.7</v>
+      </c>
+      <c r="D29">
+        <v>8.07</v>
+      </c>
+      <c r="E29">
+        <v>0.8</v>
+      </c>
+      <c r="F29">
+        <v>4.28</v>
+      </c>
+      <c r="G29">
+        <v>1.8</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>99.35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1943</v>
+      </c>
+      <c r="B30">
+        <v>47.3</v>
+      </c>
+      <c r="C30">
+        <v>1.7</v>
+      </c>
+      <c r="D30">
+        <v>32.9</v>
+      </c>
+      <c r="E30">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F30">
+        <v>18.8</v>
+      </c>
+      <c r="G30">
+        <v>2.4</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>98.999999999999986</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1944</v>
+      </c>
+      <c r="B31">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="C31">
+        <v>2.8</v>
+      </c>
+      <c r="D31">
+        <v>31.9</v>
+      </c>
+      <c r="E31">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F31">
+        <v>31.8</v>
+      </c>
+      <c r="G31">
+        <v>2.1</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>99.899999999999991</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1945</v>
+      </c>
+      <c r="B32">
+        <v>63.5</v>
+      </c>
+      <c r="C32">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D32">
+        <v>29.8</v>
+      </c>
+      <c r="E32">
+        <v>2.8</v>
+      </c>
+      <c r="F32">
+        <v>6.67</v>
+      </c>
+      <c r="G32">
+        <v>2.82</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>99.97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1946</v>
+      </c>
+      <c r="B33">
+        <v>32.4</v>
+      </c>
+      <c r="C33">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D33">
+        <v>34.4</v>
+      </c>
+      <c r="E33">
+        <v>2.5</v>
+      </c>
+      <c r="F33">
+        <v>32</v>
+      </c>
+      <c r="G33">
+        <v>4</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="0"/>
+        <v>98.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1947</v>
+      </c>
+      <c r="B34">
+        <v>49.6</v>
+      </c>
+      <c r="C34">
+        <v>1.9</v>
+      </c>
+      <c r="D34">
+        <v>17.8</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34">
+        <v>31.1</v>
+      </c>
+      <c r="G34">
+        <v>3.9</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>98.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1948</v>
+      </c>
+      <c r="B35">
+        <v>69.2</v>
+      </c>
+      <c r="C35">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D35">
+        <v>24.3</v>
+      </c>
+      <c r="E35">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F35">
+        <v>7.33</v>
+      </c>
+      <c r="G35">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>100.83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1949</v>
+      </c>
+      <c r="B36">
+        <v>50.2</v>
+      </c>
+      <c r="C36">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D36">
+        <v>30.3</v>
+      </c>
+      <c r="E36">
+        <v>2.8</v>
+      </c>
+      <c r="F36">
+        <v>20.5</v>
+      </c>
+      <c r="G36">
+        <v>3.2</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="0"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1950</v>
+      </c>
+      <c r="B37">
+        <v>48</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>35</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <v>16.3</v>
+      </c>
+      <c r="G37">
+        <v>2.7</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="0"/>
+        <v>99.3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1951</v>
+      </c>
+      <c r="B38">
+        <v>22.3</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <v>55</v>
+      </c>
+      <c r="E38">
+        <v>3.7</v>
+      </c>
+      <c r="F38">
+        <v>20.7</v>
+      </c>
+      <c r="G38">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1952</v>
+      </c>
+      <c r="B39">
+        <v>91.3</v>
+      </c>
+      <c r="C39">
+        <v>1.9</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>3.83</v>
+      </c>
+      <c r="G39">
+        <v>1.57</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="0"/>
+        <v>99.13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1953</v>
+      </c>
+      <c r="B40">
+        <v>16.3</v>
+      </c>
+      <c r="C40">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D40">
+        <v>61.3</v>
+      </c>
+      <c r="E40">
+        <v>4.3</v>
+      </c>
+      <c r="F40">
+        <v>21.4</v>
+      </c>
+      <c r="G40">
+        <v>3.7</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="0"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1954</v>
+      </c>
+      <c r="B41">
+        <v>29</v>
+      </c>
+      <c r="C41">
+        <v>3.9</v>
+      </c>
+      <c r="D41">
+        <v>40</v>
+      </c>
+      <c r="E41">
+        <v>2.7</v>
+      </c>
+      <c r="F41">
+        <v>29</v>
+      </c>
+      <c r="G41">
+        <v>2.5</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1955</v>
+      </c>
+      <c r="B42">
+        <v>41.5</v>
+      </c>
+      <c r="C42">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D42">
+        <v>30</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="F42">
+        <v>26.8</v>
+      </c>
+      <c r="G42">
+        <v>3.2</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="0"/>
+        <v>98.3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1956</v>
+      </c>
+      <c r="B43">
+        <v>28.7</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>43.9</v>
+      </c>
+      <c r="E43">
+        <v>3.7</v>
+      </c>
+      <c r="F43">
+        <v>27.1</v>
+      </c>
+      <c r="G43">
+        <v>3.4</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="0"/>
+        <v>99.699999999999989</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1957</v>
+      </c>
+      <c r="B44">
+        <v>59.6</v>
+      </c>
+      <c r="C44">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D44">
+        <v>31</v>
+      </c>
+      <c r="E44">
+        <v>3.2</v>
+      </c>
+      <c r="F44">
+        <v>7.83</v>
+      </c>
+      <c r="G44">
+        <v>2.83</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="0"/>
+        <v>98.429999999999993</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B45">
+        <v>50</v>
+      </c>
+      <c r="C45">
+        <v>1.4</v>
+      </c>
+      <c r="D45">
+        <v>18.5</v>
+      </c>
+      <c r="E45">
+        <v>2.8</v>
+      </c>
+      <c r="F45">
+        <v>31.3</v>
+      </c>
+      <c r="G45">
+        <v>3.5</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="0"/>
+        <v>99.8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1959</v>
+      </c>
+      <c r="B46">
+        <v>83.8</v>
+      </c>
+      <c r="C46">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D46">
+        <v>11</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46">
+        <v>5.42</v>
+      </c>
+      <c r="G46">
+        <v>1.85</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="0"/>
+        <v>100.22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>1960</v>
+      </c>
+      <c r="B47">
+        <v>27.9</v>
+      </c>
+      <c r="C47">
+        <v>6.7</v>
+      </c>
+      <c r="D47">
+        <v>48</v>
+      </c>
+      <c r="E47">
+        <v>6</v>
+      </c>
+      <c r="F47">
+        <v>23.6</v>
+      </c>
+      <c r="G47">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="0"/>
+        <v>99.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>1961</v>
+      </c>
+      <c r="B48">
+        <v>52.5</v>
+      </c>
+      <c r="C48">
+        <v>2.5</v>
+      </c>
+      <c r="D48">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48">
+        <v>14</v>
+      </c>
+      <c r="G48">
+        <v>2.5</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="0"/>
+        <v>99.8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>1962</v>
+      </c>
+      <c r="B49">
+        <v>26.8</v>
+      </c>
+      <c r="C49">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D49">
+        <v>64.3</v>
+      </c>
+      <c r="E49">
+        <v>6.5</v>
+      </c>
+      <c r="F49">
+        <v>7.62</v>
+      </c>
+      <c r="G49">
+        <v>2.5</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="0"/>
+        <v>98.72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>1963</v>
+      </c>
+      <c r="B50">
+        <v>51</v>
+      </c>
+      <c r="C50">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D50">
+        <v>31.3</v>
+      </c>
+      <c r="E50">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F50">
+        <v>17.3</v>
+      </c>
+      <c r="G50">
+        <v>1.7</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="0"/>
+        <v>99.6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>1964</v>
+      </c>
+      <c r="B51">
+        <v>75</v>
+      </c>
+      <c r="C51">
+        <v>1.8</v>
+      </c>
+      <c r="D51">
+        <v>16.7</v>
+      </c>
+      <c r="E51">
+        <v>1.3</v>
+      </c>
+      <c r="F51">
+        <v>7</v>
+      </c>
+      <c r="G51">
+        <v>1.6</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="0"/>
+        <v>98.7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>1965</v>
+      </c>
+      <c r="B52">
+        <v>14</v>
+      </c>
+      <c r="C52">
+        <v>2.7</v>
+      </c>
+      <c r="D52">
+        <v>62.3</v>
+      </c>
+      <c r="E52">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F52">
+        <v>25.1</v>
+      </c>
+      <c r="G52">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="0"/>
+        <v>101.4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>1966</v>
+      </c>
+      <c r="B53">
+        <v>52.1</v>
+      </c>
+      <c r="C53">
+        <v>2.1</v>
+      </c>
+      <c r="D53">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="E53">
+        <v>2.6</v>
+      </c>
+      <c r="F53">
+        <v>14.7</v>
+      </c>
+      <c r="G53">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="0"/>
+        <v>100.10000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>1967</v>
+      </c>
+      <c r="B54">
+        <v>20.3</v>
+      </c>
+      <c r="C54">
+        <v>1.8</v>
+      </c>
+      <c r="D54">
+        <v>57.8</v>
+      </c>
+      <c r="E54">
+        <v>3.6</v>
+      </c>
+      <c r="F54">
+        <v>20.9</v>
+      </c>
+      <c r="G54">
+        <v>3.6</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="0"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>1968</v>
+      </c>
+      <c r="B55">
+        <v>69.7</v>
+      </c>
+      <c r="C55">
+        <v>1.7</v>
+      </c>
+      <c r="D55">
+        <v>21.7</v>
+      </c>
+      <c r="E55">
+        <v>1.9</v>
+      </c>
+      <c r="F55">
+        <v>9.33</v>
+      </c>
+      <c r="G55">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="0"/>
+        <v>100.73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>1969</v>
+      </c>
+      <c r="B56">
+        <v>12.5</v>
+      </c>
+      <c r="C56">
+        <v>3.7</v>
+      </c>
+      <c r="D56">
+        <v>65</v>
+      </c>
+      <c r="E56">
+        <v>3.5</v>
+      </c>
+      <c r="F56">
+        <v>21.4</v>
+      </c>
+      <c r="G56">
+        <v>3.2</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="0"/>
+        <v>98.9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>1970</v>
+      </c>
+      <c r="B57">
+        <v>21</v>
+      </c>
+      <c r="C57">
+        <v>3.9</v>
+      </c>
+      <c r="D57">
+        <v>44.8</v>
+      </c>
+      <c r="E57">
+        <v>4.2</v>
+      </c>
+      <c r="F57">
+        <v>33</v>
+      </c>
+      <c r="G57">
+        <v>3.7</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="0"/>
+        <v>98.8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>1971</v>
+      </c>
+      <c r="B58">
+        <v>47</v>
+      </c>
+      <c r="C58">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D58">
+        <v>44.9</v>
+      </c>
+      <c r="E58">
+        <v>3.4</v>
+      </c>
+      <c r="F58">
+        <v>8.24</v>
+      </c>
+      <c r="G58">
+        <v>2.23</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="0"/>
+        <v>100.14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B59">
+        <v>20.8</v>
+      </c>
+      <c r="C59">
+        <v>3.2</v>
+      </c>
+      <c r="D59">
+        <v>51.6</v>
+      </c>
+      <c r="E59">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F59">
+        <v>26</v>
+      </c>
+      <c r="G59">
+        <v>5.6</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="0"/>
+        <v>98.4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>1973</v>
+      </c>
+      <c r="B60">
+        <v>70.7</v>
+      </c>
+      <c r="C60">
+        <v>1.8</v>
+      </c>
+      <c r="D60">
+        <v>20</v>
+      </c>
+      <c r="E60">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F60">
+        <v>9.19</v>
+      </c>
+      <c r="G60">
+        <v>3.4</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="0"/>
+        <v>99.89</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>1974</v>
+      </c>
+      <c r="B61">
+        <v>24.4</v>
+      </c>
+      <c r="C61">
+        <v>3.1</v>
+      </c>
+      <c r="D61">
+        <v>57</v>
+      </c>
+      <c r="E61">
+        <v>3.7</v>
+      </c>
+      <c r="F61">
+        <v>17.2</v>
+      </c>
+      <c r="G61">
+        <v>3.3</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="0"/>
+        <v>98.600000000000009</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>1975</v>
+      </c>
+      <c r="B62">
+        <v>87</v>
+      </c>
+      <c r="C62">
+        <v>1.9</v>
+      </c>
+      <c r="D62">
+        <v>7.63</v>
+      </c>
+      <c r="E62">
+        <v>1.63</v>
+      </c>
+      <c r="F62">
+        <v>6</v>
+      </c>
+      <c r="G62">
+        <v>1.96</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="0"/>
+        <v>100.63</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B63">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="C63">
+        <v>2.1</v>
+      </c>
+      <c r="D63">
+        <v>16.8</v>
+      </c>
+      <c r="E63">
+        <v>1.5</v>
+      </c>
+      <c r="F63">
+        <v>6.67</v>
+      </c>
+      <c r="G63">
+        <v>1.83</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="0"/>
+        <v>101.07</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>1977</v>
+      </c>
+      <c r="B64">
+        <v>44.7</v>
+      </c>
+      <c r="C64">
+        <v>2.5</v>
+      </c>
+      <c r="D64">
+        <v>31</v>
+      </c>
+      <c r="E64">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F64">
+        <v>25.8</v>
+      </c>
+      <c r="G64">
+        <v>3.8</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="0"/>
+        <v>101.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>1978</v>
+      </c>
+      <c r="B65">
+        <v>33</v>
+      </c>
+      <c r="C65">
+        <v>3.5</v>
+      </c>
+      <c r="D65">
+        <v>22</v>
+      </c>
+      <c r="E65">
+        <v>2</v>
+      </c>
+      <c r="F65">
+        <v>45.5</v>
+      </c>
+      <c r="G65">
+        <v>3.3</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="0"/>
+        <v>100.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>1979</v>
+      </c>
+      <c r="B66">
+        <v>55.5</v>
+      </c>
+      <c r="C66">
+        <v>1.8</v>
+      </c>
+      <c r="D66">
+        <v>27.8</v>
+      </c>
+      <c r="E66">
+        <v>3.5</v>
+      </c>
+      <c r="F66">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="G66">
+        <v>3.8</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="0"/>
+        <v>102.4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>1980</v>
+      </c>
+      <c r="B67">
+        <v>29.6</v>
+      </c>
+      <c r="C67">
+        <v>2.9</v>
+      </c>
+      <c r="D67" s="2249">
+        <v>36.4</v>
+      </c>
+      <c r="E67" s="2249">
+        <v>3.7</v>
+      </c>
+      <c r="F67" s="2249">
+        <v>29.2</v>
+      </c>
+      <c r="G67" s="2249">
+        <v>3.2</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="0"/>
+        <v>95.2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>1981</v>
+      </c>
+      <c r="B68">
+        <v>21.1</v>
+      </c>
+      <c r="C68">
+        <v>3.1</v>
+      </c>
+      <c r="D68" s="2249">
+        <v>60.2</v>
+      </c>
+      <c r="E68" s="2249">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F68" s="2249">
+        <v>22.4</v>
+      </c>
+      <c r="G68" s="2249">
+        <v>5.8</v>
+      </c>
+      <c r="I68">
+        <f t="shared" ref="I68:I71" si="1">B68+D68+F68</f>
+        <v>103.70000000000002</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>1982</v>
+      </c>
+      <c r="B69">
+        <v>49.7</v>
+      </c>
+      <c r="C69">
+        <v>1.7</v>
+      </c>
+      <c r="D69" s="2249">
+        <v>39.6</v>
+      </c>
+      <c r="E69" s="2249">
+        <v>3.4</v>
+      </c>
+      <c r="F69" s="2249">
+        <v>15</v>
+      </c>
+      <c r="G69" s="2249">
+        <v>2.9</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="1"/>
+        <v>104.30000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>1983</v>
+      </c>
+      <c r="B70">
+        <v>24.3</v>
+      </c>
+      <c r="C70">
+        <v>1.7</v>
+      </c>
+      <c r="D70" s="2249">
+        <v>54.9</v>
+      </c>
+      <c r="E70" s="2249">
+        <v>5.9</v>
+      </c>
+      <c r="F70" s="2249">
+        <v>15.2</v>
+      </c>
+      <c r="G70" s="2249">
+        <v>3.8</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="1"/>
+        <v>94.4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>1984</v>
+      </c>
+      <c r="B71">
+        <v>57.2</v>
+      </c>
+      <c r="C71">
+        <v>3.2</v>
+      </c>
+      <c r="D71" s="2249">
+        <v>33.5</v>
+      </c>
+      <c r="E71" s="2249">
+        <v>2.5</v>
+      </c>
+      <c r="F71" s="2249">
+        <v>9</v>
+      </c>
+      <c r="G71" s="2249">
+        <v>1.8</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="1"/>
+        <v>99.7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -45669,8 +47525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G864"/>
   <sheetViews>
-    <sheetView topLeftCell="A848" workbookViewId="0">
-      <selection activeCell="A854" sqref="A854:XFD857"/>
+    <sheetView topLeftCell="A841" workbookViewId="0">
+      <selection activeCell="A865" sqref="A865"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>